<commit_message>
updated Model Algo - updated projections
</commit_message>
<xml_diff>
--- a/UpdatedResultsNFL.xlsx
+++ b/UpdatedResultsNFL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aagbebaku.TSI\Documents\NFL-Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NFL-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A55C8B0-8546-46F4-B3AC-EAB24B88A836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870FB632-AD72-4123-A620-5934E41BA3A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="4" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="WL Record" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="88">
   <si>
     <t>Atlanta Falcons</t>
   </si>
@@ -259,46 +258,49 @@
     <t>Prediction Visitor</t>
   </si>
   <si>
-    <t>Miami +7.5</t>
-  </si>
-  <si>
     <t>Las Vegas +2.5</t>
   </si>
   <si>
-    <t>Philadelphia +3</t>
-  </si>
-  <si>
-    <t>Detroit +8.5</t>
-  </si>
-  <si>
     <t>Dallas - 9</t>
   </si>
   <si>
-    <t>Washington +9.5</t>
-  </si>
-  <si>
-    <t>New York Jets +12</t>
-  </si>
-  <si>
-    <t>Cleveland +2.5</t>
-  </si>
-  <si>
-    <t>Tennessee -3</t>
-  </si>
-  <si>
     <t>Indianapolis -10</t>
   </si>
   <si>
-    <t>Los Angeles -3</t>
-  </si>
-  <si>
     <t>Arizona - 10</t>
   </si>
   <si>
-    <t>Seattle +3</t>
-  </si>
-  <si>
-    <t>San Francisco +4</t>
+    <t>Baltimore -7.5</t>
+  </si>
+  <si>
+    <t>Pittsburgh -16</t>
+  </si>
+  <si>
+    <t>Tampa Bay - 9.5</t>
+  </si>
+  <si>
+    <t>Buffalo -12</t>
+  </si>
+  <si>
+    <t>New England -7</t>
+  </si>
+  <si>
+    <t>New Orleans +3</t>
+  </si>
+  <si>
+    <t>Minnesota +3</t>
+  </si>
+  <si>
+    <t>Denver -3</t>
+  </si>
+  <si>
+    <t>PUSH(Dealers Choice)</t>
+  </si>
+  <si>
+    <t>Green Bay -3</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams -4</t>
   </si>
 </sst>
 </file>
@@ -694,7 +696,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,7 +709,7 @@
     <col min="6" max="6" width="18.1796875" customWidth="1"/>
     <col min="7" max="7" width="21.81640625" customWidth="1"/>
     <col min="9" max="9" width="13.6328125" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="10" max="10" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -750,22 +752,22 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D2">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F2">
         <v>7.5</v>
       </c>
       <c r="G2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="H2">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2">
         <v>46.5</v>
@@ -782,28 +784,28 @@
         <v>25</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>8.5</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H3">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I3">
         <v>42.5</v>
       </c>
       <c r="J3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -814,22 +816,22 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4">
-        <v>-11</v>
+        <v>-15</v>
       </c>
       <c r="F4">
         <v>-9</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="H4">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I4">
         <v>55</v>
@@ -846,22 +848,22 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E5">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F5">
         <v>9.5</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H5">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I5">
         <v>51.5</v>
@@ -878,22 +880,22 @@
         <v>46</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E6">
-        <v>-10</v>
+        <v>-25</v>
       </c>
       <c r="F6">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H6">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I6">
         <v>47.5</v>
@@ -910,22 +912,22 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="F7">
         <v>-2.5</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H7">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I7">
         <v>45</v>
@@ -942,22 +944,22 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E8">
-        <v>-13</v>
+        <v>-2</v>
       </c>
       <c r="F8">
         <v>-3</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I8">
         <v>44.5</v>
@@ -977,19 +979,19 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E9">
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="F9">
         <v>-10</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H9">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I9">
         <v>47.5</v>
@@ -1006,22 +1008,22 @@
         <v>18</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10">
-        <v>-17</v>
+        <v>-18</v>
       </c>
       <c r="F10">
         <v>-10</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H10">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="I10">
         <v>44.5</v>
@@ -1041,10 +1043,10 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11">
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="F11">
         <v>-3</v>
@@ -1053,7 +1055,7 @@
         <v>83</v>
       </c>
       <c r="H11">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I11">
         <v>53</v>
@@ -1070,28 +1072,28 @@
         <v>14</v>
       </c>
       <c r="C12">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D12">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="E12">
-        <v>15</v>
+        <v>-6</v>
       </c>
       <c r="F12">
         <v>-3</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="H12">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="I12">
         <v>44</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -1102,22 +1104,22 @@
         <v>20</v>
       </c>
       <c r="C13">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E13">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="F13">
         <v>-3</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H13">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I13">
         <v>49.5</v>
@@ -1134,22 +1136,22 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>29</v>
       </c>
       <c r="E14">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="F14">
         <v>2.5</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I14">
         <v>51.5</v>
@@ -1166,19 +1168,19 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D15">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E15">
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="F15">
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H15">
         <v>55</v>

</xml_diff>

<commit_message>
added PACE calculation. Updated Proj
</commit_message>
<xml_diff>
--- a/UpdatedResultsNFL.xlsx
+++ b/UpdatedResultsNFL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NFL-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7895C3CF-7684-4706-B3CF-14E867B4C81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C547D-21CA-4E42-BF65-2D375D28C75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="4" r:id="rId1"/>
@@ -320,12 +320,6 @@
     <t>Buffalo -7</t>
   </si>
   <si>
-    <t>Minnesota -2</t>
-  </si>
-  <si>
-    <t>Baltimore -6</t>
-  </si>
-  <si>
     <t>Carolina -3.5</t>
   </si>
   <si>
@@ -344,10 +338,16 @@
     <t>Waiting on Injury Report</t>
   </si>
   <si>
-    <t>Pittsburgh +5.5</t>
-  </si>
-  <si>
     <t>Tampa Bay -11.5</t>
+  </si>
+  <si>
+    <t>Minnesota +2</t>
+  </si>
+  <si>
+    <t>Baltimore -5</t>
+  </si>
+  <si>
+    <t>Los Angeles Chargers -5.5</t>
   </si>
 </sst>
 </file>
@@ -742,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31079618-4BFE-477F-846A-6A561CEA3C78}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -834,10 +834,10 @@
         <v>27</v>
       </c>
       <c r="D3">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>6</v>
@@ -846,13 +846,13 @@
         <v>90</v>
       </c>
       <c r="H3">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I3">
         <v>45</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -863,13 +863,13 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="E4">
-        <v>-15</v>
+        <v>-20</v>
       </c>
       <c r="F4">
         <v>-7</v>
@@ -878,7 +878,7 @@
         <v>93</v>
       </c>
       <c r="H4">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="I4">
         <v>50</v>
@@ -895,22 +895,22 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F5">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="H5">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5">
         <v>49</v>
@@ -927,28 +927,28 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D6">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="F6">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="H6">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I6">
         <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -959,10 +959,10 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E7">
         <v>-11</v>
@@ -971,16 +971,16 @@
         <v>-3.5</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H7">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I7">
         <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -991,28 +991,28 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D8">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8">
-        <v>-14</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>-11.5</v>
       </c>
       <c r="G8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H8">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="I8">
         <v>43.5</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -1023,22 +1023,22 @@
         <v>22</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D9">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E9">
-        <v>-22</v>
+        <v>-33</v>
       </c>
       <c r="F9">
         <v>-10</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H9">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I9">
         <v>44.5</v>
@@ -1055,10 +1055,10 @@
         <v>17</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1067,10 +1067,10 @@
         <v>-1.5</v>
       </c>
       <c r="G10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I10">
         <v>43</v>
@@ -1087,13 +1087,13 @@
         <v>46</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11">
         <v>3</v>
@@ -1102,13 +1102,13 @@
         <v>91</v>
       </c>
       <c r="H11">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I11">
         <v>44.5</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -1119,13 +1119,13 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D12">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1134,7 +1134,7 @@
         <v>92</v>
       </c>
       <c r="H12">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I12">
         <v>49.5</v>
@@ -1151,22 +1151,22 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D13">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E13">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F13">
         <v>-2.5</v>
       </c>
       <c r="G13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H13">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="I13">
         <v>56</v>
@@ -1189,7 +1189,7 @@
         <v>2.5</v>
       </c>
       <c r="G14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1209,28 +1209,28 @@
         <v>16</v>
       </c>
       <c r="C15">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E15">
-        <v>-3</v>
+        <v>-9</v>
       </c>
       <c r="F15">
         <v>-5.5</v>
       </c>
       <c r="G15" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I15">
         <v>47</v>
       </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1241,22 +1241,22 @@
         <v>69</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D16">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="E16">
-        <v>-15</v>
+        <v>-26</v>
       </c>
       <c r="F16">
         <v>-11.5</v>
       </c>
       <c r="G16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H16">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I16">
         <v>49.5</v>
@@ -2728,7 +2728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0268A11-C6B6-4205-835F-8D0DC9D67ED8}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
lamar injury update proj
</commit_message>
<xml_diff>
--- a/UpdatedResultsNFL.xlsx
+++ b/UpdatedResultsNFL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NFL-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C547D-21CA-4E42-BF65-2D375D28C75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3ECBE-4D07-49C4-B0A2-466A0F1BD3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="4" r:id="rId1"/>
@@ -344,10 +344,10 @@
     <t>Minnesota +2</t>
   </si>
   <si>
-    <t>Baltimore -5</t>
-  </si>
-  <si>
     <t>Los Angeles Chargers -5.5</t>
+  </si>
+  <si>
+    <t>Baltimore -1.5</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -927,25 +927,25 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D6">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>18</v>
+        <v>-6</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H6">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I6">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J6" t="s">
         <v>68</v>
@@ -1221,7 +1221,7 @@
         <v>-5.5</v>
       </c>
       <c r="G15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15">
         <v>45</v>

</xml_diff>

<commit_message>
update to week 13
</commit_message>
<xml_diff>
--- a/UpdatedResultsNFL.xlsx
+++ b/UpdatedResultsNFL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NFL-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6F0555-2CFD-4771-8253-0D5F57C5769B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B75E4D-65E1-4010-910F-88D1744AF1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="134">
   <si>
     <t>Atlanta Falcons</t>
   </si>
@@ -390,6 +390,54 @@
   </si>
   <si>
     <t>Washington -1</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Dallas -4.5</t>
+  </si>
+  <si>
+    <t>Minnesota -7</t>
+  </si>
+  <si>
+    <t>Tampa Bay -11</t>
+  </si>
+  <si>
+    <t>Indianapolis -9</t>
+  </si>
+  <si>
+    <t>Philadelphia -6.5</t>
+  </si>
+  <si>
+    <t>San Francisco -3.5</t>
+  </si>
+  <si>
+    <t>Arizona -7.5</t>
+  </si>
+  <si>
+    <t>Cincinnati -3</t>
+  </si>
+  <si>
+    <t>New York Giants +5</t>
+  </si>
+  <si>
+    <t>Denver +8</t>
+  </si>
+  <si>
+    <t>Las Vegas -2.5</t>
+  </si>
+  <si>
+    <t>Los Angeles Rams -13</t>
+  </si>
+  <si>
+    <t>Baltimore -4.5</t>
+  </si>
+  <si>
+    <t>Buffalo -2.5</t>
   </si>
 </sst>
 </file>
@@ -782,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31079618-4BFE-477F-846A-6A561CEA3C78}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -835,95 +883,95 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D2">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="G2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="H2">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="I2">
-        <v>41.5</v>
+        <v>47.5</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="E3">
-        <v>-20</v>
+        <v>17</v>
       </c>
       <c r="F3">
-        <v>-7.5</v>
+        <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="H3">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="I3">
-        <v>51.5</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D4">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="H4">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4">
-        <v>45.5</v>
+        <v>50.5</v>
       </c>
       <c r="J4" t="s">
         <v>66</v>
@@ -931,159 +979,159 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D5">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E5">
-        <v>-16</v>
+        <v>27</v>
       </c>
       <c r="F5">
-        <v>-4.5</v>
+        <v>7.5</v>
       </c>
       <c r="G5" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="H5">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="I5">
-        <v>45</v>
+        <v>46.5</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E6">
-        <v>-2</v>
+        <v>26</v>
       </c>
       <c r="F6">
-        <v>-2.5</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="H6">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I6">
-        <v>44.5</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E7">
-        <v>7</v>
+        <v>-15</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="H7">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="I7">
-        <v>42</v>
+        <v>50.5</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>18</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>-4</v>
       </c>
       <c r="F8">
-        <v>3.5</v>
+        <v>-5</v>
       </c>
       <c r="G8" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="H8">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="I8">
-        <v>45.5</v>
+        <v>41.5</v>
       </c>
       <c r="J8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D9">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>-8</v>
       </c>
       <c r="F9">
-        <v>2.5</v>
+        <v>-10</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="H9">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I9">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J9" t="s">
         <v>68</v>
@@ -1091,31 +1139,31 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+      <c r="E10">
+        <v>16</v>
+      </c>
+      <c r="F10">
+        <v>6.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
         <v>45</v>
-      </c>
-      <c r="C10">
-        <v>37</v>
-      </c>
-      <c r="D10">
-        <v>35</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10">
-        <v>72</v>
-      </c>
-      <c r="I10">
-        <v>53</v>
       </c>
       <c r="J10" t="s">
         <v>66</v>
@@ -1123,31 +1171,31 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>21</v>
       </c>
       <c r="D11">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <v>-12</v>
+        <v>-9</v>
       </c>
       <c r="F11">
-        <v>-7</v>
+        <v>-2.5</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="H11">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I11">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="J11" t="s">
         <v>66</v>
@@ -1155,63 +1203,63 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>-28</v>
       </c>
       <c r="F12">
-        <v>2.5</v>
+        <v>-13</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="H12">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="I12">
         <v>48</v>
       </c>
       <c r="J12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>27</v>
+      </c>
+      <c r="D13">
         <v>20</v>
       </c>
-      <c r="C13">
-        <v>28</v>
-      </c>
-      <c r="D13">
-        <v>25</v>
-      </c>
       <c r="E13">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="G13" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="H13">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="I13">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
         <v>66</v>
@@ -1219,98 +1267,66 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
       <c r="C14">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E14">
-        <v>-3</v>
+        <v>9</v>
       </c>
       <c r="F14">
-        <v>-3</v>
+        <v>3.5</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="H14">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="I14">
-        <v>49</v>
+        <v>45.5</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E15">
-        <v>-9</v>
+        <v>-7</v>
       </c>
       <c r="F15">
-        <v>-3.5</v>
+        <v>-3</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="H15">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="I15">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J15" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>20</v>
-      </c>
-      <c r="E16">
-        <v>-1</v>
-      </c>
-      <c r="F16">
-        <v>-1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H16">
-        <v>39</v>
-      </c>
-      <c r="I16">
-        <v>46.5</v>
-      </c>
-      <c r="J16" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1320,12 +1336,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B6AE3A-BD10-4395-A680-AB7F59500C66}">
-  <dimension ref="A1:P43"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="O35" sqref="O35"/>
+      <selection pane="bottomLeft" activeCell="P44" sqref="P44:P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2770,6 +2786,9 @@
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -2817,6 +2836,9 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
       <c r="B30" t="s">
         <v>19</v>
       </c>
@@ -2864,6 +2886,9 @@
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>119</v>
+      </c>
       <c r="B31" t="s">
         <v>45</v>
       </c>
@@ -2911,6 +2936,9 @@
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>119</v>
+      </c>
       <c r="B32" t="s">
         <v>20</v>
       </c>
@@ -2957,7 +2985,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>119</v>
+      </c>
       <c r="B33" t="s">
         <v>9</v>
       </c>
@@ -3004,7 +3035,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>119</v>
+      </c>
       <c r="B34" t="s">
         <v>70</v>
       </c>
@@ -3051,7 +3085,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>119</v>
+      </c>
       <c r="B35" t="s">
         <v>67</v>
       </c>
@@ -3098,7 +3135,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
@@ -3145,7 +3185,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>119</v>
+      </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
@@ -3192,7 +3235,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>119</v>
+      </c>
       <c r="B38" t="s">
         <v>7</v>
       </c>
@@ -3239,7 +3285,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>119</v>
+      </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
@@ -3286,7 +3335,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
       <c r="B40" t="s">
         <v>15</v>
       </c>
@@ -3333,7 +3385,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>119</v>
+      </c>
       <c r="B41" t="s">
         <v>18</v>
       </c>
@@ -3380,7 +3435,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>119</v>
+      </c>
       <c r="B42" t="s">
         <v>25</v>
       </c>
@@ -3427,7 +3485,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>119</v>
+      </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
@@ -3472,6 +3533,756 @@
       </c>
       <c r="P43" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44">
+        <v>16</v>
+      </c>
+      <c r="E44">
+        <v>14</v>
+      </c>
+      <c r="F44">
+        <v>13</v>
+      </c>
+      <c r="G44">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
+        <v>52</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>3</v>
+      </c>
+      <c r="K44">
+        <v>26</v>
+      </c>
+      <c r="L44">
+        <v>41.5</v>
+      </c>
+      <c r="M44">
+        <v>30</v>
+      </c>
+      <c r="N44" t="s">
+        <v>104</v>
+      </c>
+      <c r="O44" t="s">
+        <v>68</v>
+      </c>
+      <c r="P44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>36</v>
+      </c>
+      <c r="E45">
+        <v>33</v>
+      </c>
+      <c r="F45">
+        <v>20</v>
+      </c>
+      <c r="G45">
+        <v>40</v>
+      </c>
+      <c r="H45" t="s">
+        <v>53</v>
+      </c>
+      <c r="I45">
+        <v>-20</v>
+      </c>
+      <c r="J45">
+        <v>-7.5</v>
+      </c>
+      <c r="K45">
+        <v>60</v>
+      </c>
+      <c r="L45">
+        <v>51.5</v>
+      </c>
+      <c r="M45">
+        <v>69</v>
+      </c>
+      <c r="N45" t="s">
+        <v>108</v>
+      </c>
+      <c r="O45" t="s">
+        <v>66</v>
+      </c>
+      <c r="P45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>31</v>
+      </c>
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>34</v>
+      </c>
+      <c r="G46">
+        <v>25</v>
+      </c>
+      <c r="H46" t="s">
+        <v>52</v>
+      </c>
+      <c r="I46">
+        <v>9</v>
+      </c>
+      <c r="J46">
+        <v>6</v>
+      </c>
+      <c r="K46">
+        <v>59</v>
+      </c>
+      <c r="L46">
+        <v>45.5</v>
+      </c>
+      <c r="M46">
+        <v>37</v>
+      </c>
+      <c r="N46" t="s">
+        <v>109</v>
+      </c>
+      <c r="O46" t="s">
+        <v>66</v>
+      </c>
+      <c r="P46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+      <c r="E47">
+        <v>41</v>
+      </c>
+      <c r="F47">
+        <v>18</v>
+      </c>
+      <c r="G47">
+        <v>34</v>
+      </c>
+      <c r="H47" t="s">
+        <v>52</v>
+      </c>
+      <c r="I47">
+        <v>-16</v>
+      </c>
+      <c r="J47">
+        <v>-4.5</v>
+      </c>
+      <c r="K47">
+        <v>52</v>
+      </c>
+      <c r="L47">
+        <v>45</v>
+      </c>
+      <c r="M47">
+        <v>51</v>
+      </c>
+      <c r="N47" t="s">
+        <v>112</v>
+      </c>
+      <c r="O47" t="s">
+        <v>66</v>
+      </c>
+      <c r="P47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>21</v>
+      </c>
+      <c r="E48">
+        <v>14</v>
+      </c>
+      <c r="F48">
+        <v>17</v>
+      </c>
+      <c r="G48">
+        <v>19</v>
+      </c>
+      <c r="H48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48">
+        <v>-2</v>
+      </c>
+      <c r="J48">
+        <v>-2.5</v>
+      </c>
+      <c r="K48">
+        <v>36</v>
+      </c>
+      <c r="L48">
+        <v>44.5</v>
+      </c>
+      <c r="M48">
+        <v>35</v>
+      </c>
+      <c r="N48" t="s">
+        <v>114</v>
+      </c>
+      <c r="O48" t="s">
+        <v>68</v>
+      </c>
+      <c r="P48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>33</v>
+      </c>
+      <c r="F49">
+        <v>19</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49">
+        <v>7</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>31</v>
+      </c>
+      <c r="L49">
+        <v>42</v>
+      </c>
+      <c r="M49">
+        <v>43</v>
+      </c>
+      <c r="N49" t="s">
+        <v>115</v>
+      </c>
+      <c r="O49" t="s">
+        <v>68</v>
+      </c>
+      <c r="P49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>118</v>
+      </c>
+      <c r="B50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50">
+        <v>7</v>
+      </c>
+      <c r="E50">
+        <v>13</v>
+      </c>
+      <c r="F50">
+        <v>30</v>
+      </c>
+      <c r="G50">
+        <v>18</v>
+      </c>
+      <c r="H50" t="s">
+        <v>53</v>
+      </c>
+      <c r="I50">
+        <v>12</v>
+      </c>
+      <c r="J50">
+        <v>3.5</v>
+      </c>
+      <c r="K50">
+        <v>48</v>
+      </c>
+      <c r="L50">
+        <v>45.5</v>
+      </c>
+      <c r="M50">
+        <v>20</v>
+      </c>
+      <c r="N50" t="s">
+        <v>110</v>
+      </c>
+      <c r="O50" t="s">
+        <v>66</v>
+      </c>
+      <c r="P50" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>21</v>
+      </c>
+      <c r="E51">
+        <v>14</v>
+      </c>
+      <c r="F51">
+        <v>16</v>
+      </c>
+      <c r="G51">
+        <v>17</v>
+      </c>
+      <c r="H51" t="s">
+        <v>53</v>
+      </c>
+      <c r="I51">
+        <v>-1</v>
+      </c>
+      <c r="J51">
+        <v>2.5</v>
+      </c>
+      <c r="K51">
+        <v>33</v>
+      </c>
+      <c r="L51">
+        <v>46</v>
+      </c>
+      <c r="M51">
+        <v>35</v>
+      </c>
+      <c r="N51" t="s">
+        <v>105</v>
+      </c>
+      <c r="O51" t="s">
+        <v>68</v>
+      </c>
+      <c r="P51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D52">
+        <v>38</v>
+      </c>
+      <c r="E52">
+        <v>31</v>
+      </c>
+      <c r="F52">
+        <v>37</v>
+      </c>
+      <c r="G52">
+        <v>35</v>
+      </c>
+      <c r="H52" t="s">
+        <v>53</v>
+      </c>
+      <c r="I52">
+        <v>2</v>
+      </c>
+      <c r="J52">
+        <v>3</v>
+      </c>
+      <c r="K52">
+        <v>72</v>
+      </c>
+      <c r="L52">
+        <v>53</v>
+      </c>
+      <c r="M52">
+        <v>69</v>
+      </c>
+      <c r="N52" t="s">
+        <v>106</v>
+      </c>
+      <c r="O52" t="s">
+        <v>66</v>
+      </c>
+      <c r="P52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>13</v>
+      </c>
+      <c r="E53">
+        <v>36</v>
+      </c>
+      <c r="F53">
+        <v>21</v>
+      </c>
+      <c r="G53">
+        <v>33</v>
+      </c>
+      <c r="H53" t="s">
+        <v>52</v>
+      </c>
+      <c r="I53">
+        <v>-12</v>
+      </c>
+      <c r="J53">
+        <v>-7</v>
+      </c>
+      <c r="K53">
+        <v>54</v>
+      </c>
+      <c r="L53">
+        <v>44</v>
+      </c>
+      <c r="M53">
+        <v>49</v>
+      </c>
+      <c r="N53" t="s">
+        <v>81</v>
+      </c>
+      <c r="O53" t="s">
+        <v>66</v>
+      </c>
+      <c r="P53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>13</v>
+      </c>
+      <c r="E54">
+        <v>28</v>
+      </c>
+      <c r="F54">
+        <v>25</v>
+      </c>
+      <c r="G54">
+        <v>24</v>
+      </c>
+      <c r="H54" t="s">
+        <v>52</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>2.5</v>
+      </c>
+      <c r="K54">
+        <v>49</v>
+      </c>
+      <c r="L54">
+        <v>48</v>
+      </c>
+      <c r="M54">
+        <v>41</v>
+      </c>
+      <c r="N54" t="s">
+        <v>107</v>
+      </c>
+      <c r="O54" t="s">
+        <v>66</v>
+      </c>
+      <c r="P54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>118</v>
+      </c>
+      <c r="B55" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" t="s">
+        <v>20</v>
+      </c>
+      <c r="D55">
+        <v>28</v>
+      </c>
+      <c r="E55">
+        <v>36</v>
+      </c>
+      <c r="F55">
+        <v>28</v>
+      </c>
+      <c r="G55">
+        <v>25</v>
+      </c>
+      <c r="H55" t="s">
+        <v>53</v>
+      </c>
+      <c r="I55">
+        <v>3</v>
+      </c>
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>53</v>
+      </c>
+      <c r="L55">
+        <v>47</v>
+      </c>
+      <c r="M55">
+        <v>64</v>
+      </c>
+      <c r="N55" t="s">
+        <v>116</v>
+      </c>
+      <c r="O55" t="s">
+        <v>66</v>
+      </c>
+      <c r="P55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56">
+        <v>26</v>
+      </c>
+      <c r="E56">
+        <v>34</v>
+      </c>
+      <c r="F56">
+        <v>26</v>
+      </c>
+      <c r="G56">
+        <v>29</v>
+      </c>
+      <c r="H56" t="s">
+        <v>52</v>
+      </c>
+      <c r="I56">
+        <v>-3</v>
+      </c>
+      <c r="J56">
+        <v>-3</v>
+      </c>
+      <c r="K56">
+        <v>55</v>
+      </c>
+      <c r="L56">
+        <v>49</v>
+      </c>
+      <c r="M56">
+        <v>60</v>
+      </c>
+      <c r="N56" t="s">
+        <v>111</v>
+      </c>
+      <c r="O56" t="s">
+        <v>66</v>
+      </c>
+      <c r="P56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+      <c r="E57">
+        <v>16</v>
+      </c>
+      <c r="F57">
+        <v>21</v>
+      </c>
+      <c r="G57">
+        <v>30</v>
+      </c>
+      <c r="H57" t="s">
+        <v>52</v>
+      </c>
+      <c r="I57">
+        <v>-9</v>
+      </c>
+      <c r="J57">
+        <v>-3.5</v>
+      </c>
+      <c r="K57">
+        <v>51</v>
+      </c>
+      <c r="L57">
+        <v>46</v>
+      </c>
+      <c r="M57">
+        <v>26</v>
+      </c>
+      <c r="N57" t="s">
+        <v>113</v>
+      </c>
+      <c r="O57" t="s">
+        <v>66</v>
+      </c>
+      <c r="P57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>118</v>
+      </c>
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58">
+        <v>15</v>
+      </c>
+      <c r="E58">
+        <v>17</v>
+      </c>
+      <c r="F58">
+        <v>19</v>
+      </c>
+      <c r="G58">
+        <v>20</v>
+      </c>
+      <c r="H58" t="s">
+        <v>52</v>
+      </c>
+      <c r="I58">
+        <v>-1</v>
+      </c>
+      <c r="J58">
+        <v>-1</v>
+      </c>
+      <c r="K58">
+        <v>39</v>
+      </c>
+      <c r="L58">
+        <v>46.5</v>
+      </c>
+      <c r="M58">
+        <v>32</v>
+      </c>
+      <c r="N58" t="s">
+        <v>117</v>
+      </c>
+      <c r="O58" t="s">
+        <v>68</v>
+      </c>
+      <c r="P58" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -3484,7 +4295,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3519,27 +4330,27 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>COUNTIF(Results!H2:H72,"WIN")</f>
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <f>COUNTIF(Results!H2:H72,"LOSS")</f>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <f>ROUND(SUM(A2/(A2+B2)),3)</f>
-        <v>0.45200000000000001</v>
+        <v>0.49099999999999999</v>
       </c>
       <c r="D2">
         <f>COUNTIF(Results!P2:P72,"WIN")</f>
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E2">
         <f>COUNTIF(Results!P2:P72,"LOSS")</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F2">
         <f>ROUND(SUM(D2/(D2+E2)),3)</f>
-        <v>0.42899999999999999</v>
+        <v>0.49099999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update lines and injuries
</commit_message>
<xml_diff>
--- a/UpdatedResultsNFL.xlsx
+++ b/UpdatedResultsNFL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\NFL-Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B75E4D-65E1-4010-910F-88D1744AF1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B207F1-4DF6-4144-B016-E8C00C5F0A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
+    <workbookView xWindow="-28920" yWindow="1290" windowWidth="29040" windowHeight="15840" xr2:uid="{E355D2B9-20BB-4A06-AC71-876CAB97FF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Predictions" sheetId="4" r:id="rId1"/>
@@ -410,9 +410,6 @@
     <t>Indianapolis -9</t>
   </si>
   <si>
-    <t>Philadelphia -6.5</t>
-  </si>
-  <si>
     <t>San Francisco -3.5</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
     <t>Cincinnati -3</t>
   </si>
   <si>
-    <t>New York Giants +5</t>
-  </si>
-  <si>
     <t>Denver +8</t>
   </si>
   <si>
@@ -438,6 +432,12 @@
   </si>
   <si>
     <t>Buffalo -2.5</t>
+  </si>
+  <si>
+    <t>Philadelphia -5.5</t>
+  </si>
+  <si>
+    <t>Miami -6.5</t>
   </si>
 </sst>
 </file>
@@ -833,7 +833,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,7 +939,7 @@
         <v>45</v>
       </c>
       <c r="I3">
-        <v>47</v>
+        <v>47.5</v>
       </c>
       <c r="J3" t="s">
         <v>68</v>
@@ -997,7 +997,7 @@
         <v>7.5</v>
       </c>
       <c r="G5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H5">
         <v>41</v>
@@ -1061,7 +1061,7 @@
         <v>-3</v>
       </c>
       <c r="G7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7">
         <v>65</v>
@@ -1081,19 +1081,19 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>18</v>
       </c>
       <c r="E8">
-        <v>-4</v>
+        <v>-14</v>
       </c>
       <c r="F8">
-        <v>-5</v>
+        <v>-6.5</v>
       </c>
       <c r="G8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="H8">
         <v>32</v>
@@ -1125,7 +1125,7 @@
         <v>-10</v>
       </c>
       <c r="G9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H9">
         <v>44</v>
@@ -1145,7 +1145,7 @@
         <v>46</v>
       </c>
       <c r="C10">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>17</v>
@@ -1154,16 +1154,16 @@
         <v>16</v>
       </c>
       <c r="F10">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="G10" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="H10">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I10">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
         <v>66</v>
@@ -1189,7 +1189,7 @@
         <v>-2.5</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H11">
         <v>51</v>
@@ -1221,7 +1221,7 @@
         <v>-13</v>
       </c>
       <c r="G12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H12">
         <v>46</v>
@@ -1253,7 +1253,7 @@
         <v>4.5</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H13">
         <v>47</v>
@@ -1285,7 +1285,7 @@
         <v>3.5</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H14">
         <v>41</v>
@@ -1317,7 +1317,7 @@
         <v>-3</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H15">
         <v>57</v>

</xml_diff>